<commit_message>
May 8 csv updates
</commit_message>
<xml_diff>
--- a/status/excel/fromBox/EMSX_excel.xlsx
+++ b/status/excel/fromBox/EMSX_excel.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27615"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_496DC3F7026B660F623554765845D63AAE4D9B99" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3773504E-ECA3-4793-A6D5-509CD8DEA817}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/selenawallace/Downloads/Status Sheets-selected (6)/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71DB0E06-7399-7347-AFDB-2E75AF45E1A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -163,7 +168,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -175,6 +183,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -212,12 +221,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,16 +535,16 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -542,10 +554,10 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -564,7 +576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>0</v>
       </c>
@@ -574,14 +586,14 @@
       <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -591,14 +603,14 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -608,14 +620,14 @@
       <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -625,14 +637,14 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -642,14 +654,14 @@
       <c r="C6" t="s">
         <v>11</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -659,14 +671,14 @@
       <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -676,14 +688,14 @@
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -693,14 +705,14 @@
       <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -710,14 +722,14 @@
       <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -727,14 +739,14 @@
       <c r="C11" t="s">
         <v>11</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -744,14 +756,14 @@
       <c r="C12" t="s">
         <v>11</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -761,14 +773,14 @@
       <c r="C13" t="s">
         <v>11</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E13" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -778,14 +790,14 @@
       <c r="C14" t="s">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -795,14 +807,14 @@
       <c r="C15" t="s">
         <v>11</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -812,14 +824,14 @@
       <c r="C16" t="s">
         <v>11</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E16" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -829,14 +841,14 @@
       <c r="C17" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="3">
         <v>45109</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>45291</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -846,10 +858,10 @@
       <c r="C18" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>45292</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>45366</v>
       </c>
     </row>

</xml_diff>